<commit_message>
- ADD: Added Germinate, James Hutton Institute and ICS logo to the bottom of the about Germinate page. - CHG: Converted the about Germinate page into the UiBinder framework. - CHG: Slightly changed the trials template to have a dropdown box for the unit type. This change is backwards compatible, i.e. the importer code will still work with the old templates.
</commit_message>
<xml_diff>
--- a/datatemplates/trials-data.xlsx
+++ b/datatemplates/trials-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\web-intellij\germinate3-bootstrap\datatemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\web-intellij\germinate\datatemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1A7273-7DF2-4656-947B-52E2BE182B28}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1867D2FF-D299-4BE3-AAB6-3F3DF3D4BE66}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="METADATA" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -268,6 +268,15 @@
   </si>
   <si>
     <t>The 2 letter country code of the institution (ISO 3166-1 alpha-2).</t>
+  </si>
+  <si>
+    <t>Possible data types</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>char</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1197,8 +1206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C867D861-9536-4856-8988-38BB3B3563D5}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1320,10 +1329,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,7 +1346,7 @@
     <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1359,8 +1368,11 @@
       <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1368,8 +1380,11 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -1377,8 +1392,11 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -1386,16 +1404,21 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
+      <c r="J4" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="7">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Phenotype Name" prompt="This should be the full name of the phenotype that has been scored." sqref="A1" xr:uid="{53C12F0B-3F9F-48BF-B0F0-E08B964BA4CC}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Phenotype Short Name" prompt="This is should be a shortened version of the phenotype name. This is used on some of the Germinate pages which use tables so that the phenotype name fits." sqref="B1" xr:uid="{8C19ED97-A603-4BB6-A206-2A716846C37F}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Phenotype Description" prompt="This should be a full description of the phenotype. There is no limit to the length of text that can be used here so please be descriptive." sqref="C1" xr:uid="{F089AE66-013F-4735-81BE-5882571D1849}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Data Type" prompt="This should be either 'char' for character data, 'int' for integer data (whole numbers no decimal places) and 'float' for floating point numbers." sqref="D1" xr:uid="{A6ED4372-47F5-459B-80DA-BDA21DAD41B6}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Name" prompt="The name of the unit that is defined. Examples would include 'centimetre' or 'litre'" sqref="E1" xr:uid="{812908F9-58E0-44B7-8D9B-8F24F8373A14}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Abbreviation" prompt="Abbreviation for unit. Examples include 'l' or 'cm'" sqref="F1" xr:uid="{240F401A-C0EB-48A0-9B93-B4062FF9E866}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Unit Description" prompt="A description of the unit." sqref="G1" xr:uid="{6BD03C10-201D-4FCC-A927-CC3E06375029}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{82E3529B-0246-482A-A1C4-DA13B1AEE9F4}">
+      <formula1>$J$2:$J$4</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>